<commit_message>
removed the mean calculation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMARTlabUSER\OneDrive - George Mason University - O365 Production\Documents 1\Git Hub\VSCODE\Tug_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BD6253-5371-4ADE-B8AE-98FE133D9FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA167045-46E5-4CC7-8CCE-67DD4E8BAFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="71">
   <si>
     <t>Trial</t>
   </si>
@@ -233,9 +233,6 @@
   </si>
   <si>
     <t>ST</t>
-  </si>
-  <si>
-    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -637,20 +634,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.109375" customWidth="1"/>
+    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -2239,26 +2238,6 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62">
-        <v>10.2285</v>
-      </c>
-      <c r="C62">
-        <v>0.99216666666666675</v>
-      </c>
-      <c r="D62">
-        <v>2.1638333333333342</v>
-      </c>
-      <c r="E62">
-        <v>0.1001948371812873</v>
-      </c>
-      <c r="F62">
-        <v>0.217579142551869</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>